<commit_message>
separate module to simulate YT combinations for 32 biorefineries
</commit_message>
<xml_diff>
--- a/fermentation_insights/TRY_results/a_coeff_baselines_percentiles.xlsx
+++ b/fermentation_insights/TRY_results/a_coeff_baselines_percentiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\fermentation_insights\fermentation_insights\TRY_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2592A58B-F771-4E92-97DF-12225B5E54BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E791B1AD-1BC5-4B91-A557-B169CC330E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,10 +59,10 @@
     <t>glucose</t>
   </si>
   <si>
+    <t>cornstover</t>
+  </si>
+  <si>
     <t>sugarcane</t>
-  </si>
-  <si>
-    <t>cornstover</t>
   </si>
   <si>
     <t>corn</t>
@@ -108,18 +108,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -150,7 +144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,12 +154,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,14 +460,15 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" customWidth="1"/>
     <col min="4" max="6" width="8.7265625" style="3"/>
+    <col min="8" max="8" width="8.7265625" style="4"/>
+    <col min="12" max="12" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -498,7 +487,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -513,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="3">
-        <v>-9.8824605540148047E-2</v>
+        <v>-9.3679450683223572E-2</v>
       </c>
       <c r="E2" s="3">
         <v>-9.2582264071253834E-2</v>
@@ -521,63 +510,41 @@
       <c r="F2" s="3">
         <v>0.18752000974371591</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
+        <f>ABS(D2-D$2)/D$2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="L2" s="3">
         <v>4.3366435929635197E-2</v>
       </c>
-      <c r="I2">
-        <f>IF(E2&lt;D2,IF(F2&gt;D2,1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="4">
-        <f>1-D2/D$2</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
-        <f t="shared" ref="K2:L5" si="0">1-E2/E$2</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
-        <v>7.9922838689076778E-2</v>
-      </c>
-      <c r="E3" s="7">
-        <v>-2.390221027693628E-2</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.37393064420103023</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.18921810643784959</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I25" si="1">IF(E3&lt;D3,IF(F3&gt;D3,1,0),0)</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="8">
-        <f t="shared" ref="J3:J5" si="2">1-D3/D$2</f>
-        <v>1.8087342039185543</v>
-      </c>
-      <c r="K3" s="8">
-        <f t="shared" si="0"/>
-        <v>0.74182733035627124</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" si="0"/>
-        <v>-0.9940839631572238</v>
+      <c r="D3" s="3">
+        <v>-0.13073398809803979</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-0.14738255124807201</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.1632184050975137</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:J5" si="0">ABS(D3-D$2)/D$2</f>
+        <v>-0.39554605780210955</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="L3" s="3">
+        <v>1.483511389322179E-2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -591,32 +558,21 @@
         <v>9</v>
       </c>
       <c r="D4" s="3">
-        <v>-0.1035624620383961</v>
+        <v>6.4529275980563752E-2</v>
       </c>
       <c r="E4" s="3">
-        <v>-6.636283266382631E-2</v>
+        <v>-2.390221027693628E-2</v>
       </c>
       <c r="F4" s="3">
-        <v>0.22833455956170351</v>
-      </c>
-      <c r="H4" s="3">
-        <v>9.859972807136215E-2</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <f t="shared" si="2"/>
-        <v>-4.7942073457842183E-2</v>
-      </c>
-      <c r="K4" s="4">
-        <f t="shared" si="0"/>
-        <v>0.28320144976416151</v>
-      </c>
-      <c r="L4" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.21765437125226761</v>
+        <v>0.37393064420103023</v>
+      </c>
+      <c r="H4" s="4">
+        <f>ABS(D4-D$2)/D$2</f>
+        <v>-1.6888306401237243</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="L4" s="3">
+        <v>0.18921810643784959</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -630,7 +586,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="3">
-        <v>-0.1048906526939955</v>
+        <v>-0.1227162175344394</v>
       </c>
       <c r="E5" s="3">
         <v>-0.1475885349498943</v>
@@ -638,24 +594,13 @@
       <c r="F5" s="3">
         <v>0.16954615699413031</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.3099587651234576</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="L5" s="3">
         <v>2.1029126714417451E-2</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J5" s="4">
-        <f>1-D5/D$2</f>
-        <v>-6.1381951596893414E-2</v>
-      </c>
-      <c r="K5" s="4">
-        <f t="shared" si="0"/>
-        <v>-0.5941339999668418</v>
-      </c>
-      <c r="L5" s="4">
-        <f t="shared" si="0"/>
-        <v>9.5850318982760863E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -669,7 +614,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="3">
-        <v>1.932046158381358</v>
+        <v>1.5719062716477139</v>
       </c>
       <c r="E6" s="3">
         <v>1.326342242695129</v>
@@ -677,63 +622,41 @@
       <c r="F6" s="3">
         <v>2.1720917641676021</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
+        <f>ABS(D6-D$6)/D$6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="L6" s="3">
         <v>1.709420025734383</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J6" s="4">
-        <f>1-D6/D$6</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <f t="shared" ref="K6:L9" si="3">1-E6/E$6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7">
-        <v>2.8878310756629988</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1.7530355944488261</v>
-      </c>
-      <c r="F7" s="7">
-        <v>3.3369194623680629</v>
-      </c>
-      <c r="H7" s="7">
-        <v>2.4297023194806311</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J7" s="8">
-        <f t="shared" ref="J7:J9" si="4">1-D7/D$6</f>
-        <v>-0.49470087095765058</v>
-      </c>
-      <c r="K7" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.32170682499462244</v>
-      </c>
-      <c r="L7" s="8">
-        <f t="shared" si="3"/>
-        <v>-0.53627002202038687</v>
+      <c r="D7" s="3">
+        <v>1.5188567500392409</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.155438347705029</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.0501010718874642</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" ref="H7:J9" si="1">ABS(D7-D$6)/D$6</f>
+        <v>3.3748527227940292E-2</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="L7" s="3">
+        <v>1.5572450109589611</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -747,32 +670,21 @@
         <v>9</v>
       </c>
       <c r="D8" s="3">
-        <v>1.792466003767875</v>
+        <v>2.403508314691063</v>
       </c>
       <c r="E8" s="3">
-        <v>1.155438347705029</v>
+        <v>1.5116723342073479</v>
       </c>
       <c r="F8" s="3">
-        <v>2.0501010718874642</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1.5572450109589611</v>
-      </c>
-      <c r="I8">
+        <v>3.120486416925432</v>
+      </c>
+      <c r="H8" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="4"/>
-        <v>7.2244730804165269E-2</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="3"/>
-        <v>0.12885354133245663</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="3"/>
-        <v>5.6162770971551312E-2</v>
+        <v>0.52904047654930575</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="L8" s="3">
+        <v>2.193270698269715</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -786,32 +698,21 @@
         <v>10</v>
       </c>
       <c r="D9" s="3">
-        <v>1.840367071388318</v>
+        <v>1.758467759808986</v>
       </c>
       <c r="E9" s="3">
-        <v>1.188028892018379</v>
+        <v>1.188028884180534</v>
       </c>
       <c r="F9" s="3">
-        <v>2.0756075641222842</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1.6000607801904509</v>
-      </c>
-      <c r="I9">
+        <v>2.0756075565134822</v>
+      </c>
+      <c r="H9" s="4">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="4"/>
-        <v>4.7451809883179763E-2</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="3"/>
-        <v>0.10428179562139039</v>
-      </c>
-      <c r="L9" s="4">
-        <f t="shared" si="3"/>
-        <v>4.4419946540468991E-2</v>
+        <v>0.11868486787428702</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="L9" s="3">
+        <v>1.6000607759843199</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -825,7 +726,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="3">
-        <v>0.12749387708350829</v>
+        <v>0.1183744012666984</v>
       </c>
       <c r="E10" s="3">
         <v>0.11639880465853659</v>
@@ -833,63 +734,41 @@
       <c r="F10" s="3">
         <v>0.16309943658345519</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
+        <f>ABS(D10-D$10)/D$10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="L10" s="3">
         <v>0.13960211503919689</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J10" s="4">
-        <f>1-D10/D$10</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <f t="shared" ref="K10:L13" si="5">1-E10/E$10</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="7">
-        <v>0.22547211529057079</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0.17110117431471689</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0.2887127721721624</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0.22485919207229371</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J11" s="8">
-        <f>1-D11/D$10</f>
-        <v>-0.76849367552676195</v>
-      </c>
-      <c r="K11" s="8">
-        <f t="shared" si="5"/>
-        <v>-0.46995645545204034</v>
-      </c>
-      <c r="L11" s="8">
-        <f t="shared" si="5"/>
-        <v>-0.77016412944156931</v>
+      <c r="D11" s="3">
+        <v>0.1089814407458168</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.2765481537090768E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.1785454442557752</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" ref="H11:J13" si="2">ABS(D11-D$10)/D$10</f>
+        <v>7.934959265153281E-2</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="L11" s="3">
+        <v>0.1230408527731542</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -903,32 +782,21 @@
         <v>9</v>
       </c>
       <c r="D12" s="3">
-        <v>0.11274191328236199</v>
+        <v>0.23280644402155129</v>
       </c>
       <c r="E12" s="3">
-        <v>7.2765481537090768E-2</v>
+        <v>0.17110117431471689</v>
       </c>
       <c r="F12" s="3">
-        <v>0.1785454442557752</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.1230408527731542</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" ref="J12:J13" si="6">1-D12/D$10</f>
-        <v>0.11570723346568068</v>
-      </c>
-      <c r="K12" s="4">
-        <f t="shared" si="5"/>
-        <v>0.37486057738691558</v>
-      </c>
-      <c r="L12" s="4">
-        <f t="shared" si="5"/>
-        <v>-9.4703010604310522E-2</v>
+        <v>0.2887127721721624</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.96669585256897428</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="L12" s="3">
+        <v>0.22485919207229371</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -942,7 +810,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="3">
-        <v>0.1044484247359561</v>
+        <v>0.12896284014939591</v>
       </c>
       <c r="E13" s="3">
         <v>8.0934804454870474E-2</v>
@@ -950,24 +818,13 @@
       <c r="F13" s="3">
         <v>0.13708712600488121</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
+        <v>8.9448721762416125E-2</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="L13" s="3">
         <v>0.10874761191708709</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="6"/>
-        <v>0.18075732634954267</v>
-      </c>
-      <c r="K13" s="4">
-        <f t="shared" si="5"/>
-        <v>0.30467667007150168</v>
-      </c>
-      <c r="L13" s="4">
-        <f t="shared" si="5"/>
-        <v>0.15948743369977203</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -981,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="3">
-        <v>0.30795327965375341</v>
+        <v>0.30444804553287008</v>
       </c>
       <c r="E14" s="3">
         <v>0.28723278546717301</v>
@@ -989,63 +846,41 @@
       <c r="F14" s="3">
         <v>0.35736231820904207</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
+        <f>ABS(D14-D$14)/D$14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="L14" s="3">
         <v>0.32173065524807959</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J14" s="4">
-        <f>1-D14/D$14</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <f t="shared" ref="K14:L17" si="7">1-E14/E$14</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7">
-        <v>0.42492667833145131</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0.36873876916709131</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0.5005109564506498</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0.43432624645576901</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J15" s="8">
-        <f t="shared" ref="J15:J17" si="8">1-D15/D$14</f>
-        <v>-0.37984137986520783</v>
-      </c>
-      <c r="K15" s="8">
-        <f t="shared" si="7"/>
-        <v>-0.28376281477531173</v>
-      </c>
-      <c r="L15" s="8">
-        <f t="shared" si="7"/>
-        <v>-0.40057004039768884</v>
+      <c r="D15" s="3">
+        <v>0.30095404644506202</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.2528471797025274</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.36978440765437931</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" ref="H15:J17" si="3">ABS(D15-D$14)/D$14</f>
+        <v>1.1476503590924943E-2</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="L15" s="3">
+        <v>0.3052494868683896</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -1059,32 +894,21 @@
         <v>9</v>
       </c>
       <c r="D16" s="3">
-        <v>0.29958287730066241</v>
+        <v>0.42766667654199558</v>
       </c>
       <c r="E16" s="3">
-        <v>0.2528471797025274</v>
+        <v>0.36873876916709131</v>
       </c>
       <c r="F16" s="3">
-        <v>0.36978440765437931</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.3052494868683896</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="8"/>
-        <v>2.7180754049777378E-2</v>
-      </c>
-      <c r="K16" s="4">
-        <f t="shared" si="7"/>
-        <v>0.11971337362731327</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="7"/>
-        <v>-3.4760490438924263E-2</v>
+        <v>0.5005109564506498</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.40472794231100445</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="L16" s="3">
+        <v>0.43432624645576901</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -1098,7 +922,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="3">
-        <v>0.29410073256457248</v>
+        <v>0.31736926676797489</v>
       </c>
       <c r="E17" s="3">
         <v>0.25727754571412648</v>
@@ -1106,24 +930,13 @@
       <c r="F17" s="3">
         <v>0.33458567805452938</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
+        <f t="shared" si="3"/>
+        <v>4.2441465546244582E-2</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="L17" s="3">
         <v>0.29250827781347832</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="8"/>
-        <v>4.4982625626705519E-2</v>
-      </c>
-      <c r="K17" s="4">
-        <f t="shared" si="7"/>
-        <v>0.10428906889694189</v>
-      </c>
-      <c r="L17" s="4">
-        <f t="shared" si="7"/>
-        <v>6.3735427586937954E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -1137,71 +950,49 @@
         <v>7</v>
       </c>
       <c r="D18" s="3">
-        <v>0.19741592434605851</v>
+        <v>0.20704307711349179</v>
       </c>
       <c r="E18" s="3">
-        <v>0.19256773953335149</v>
+        <v>0.20010670590599219</v>
       </c>
       <c r="F18" s="3">
-        <v>0.249436355217415</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.21953986106313189</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J18" s="4">
-        <f>1-D18/D$18</f>
+        <v>0.25899092770622861</v>
+      </c>
+      <c r="H18" s="4">
+        <f>ABS(D18-D$18)/D$18</f>
         <v>0</v>
       </c>
-      <c r="K18" s="4">
-        <f t="shared" ref="K18:L21" si="9">1-E18/E$18</f>
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5">
+      <c r="I18" s="4"/>
+      <c r="L18" s="3">
+        <v>0.22807200548761011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="7">
-        <v>0.37129146838645077</v>
-      </c>
-      <c r="E19" s="7">
-        <v>0.33313979193804211</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0.49237289417074448</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0.40276559779281301</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J19" s="8">
-        <f t="shared" ref="J19:J21" si="10">1-D19/D$18</f>
-        <v>-0.88075743948395302</v>
-      </c>
-      <c r="K19" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.72998755007115013</v>
-      </c>
-      <c r="L19" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.9739419850870572</v>
+      <c r="D19" s="3">
+        <v>0.26527888264549088</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.16133102940630159</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.34272909003202667</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" ref="H19:J21" si="4">ABS(D19-D$18)/D$18</f>
+        <v>0.28127386022222234</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="L19" s="3">
+        <v>0.25919175253236237</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -1215,32 +1006,21 @@
         <v>9</v>
       </c>
       <c r="D20" s="3">
-        <v>0.25689235231426721</v>
+        <v>0.39150567177913542</v>
       </c>
       <c r="E20" s="3">
-        <v>0.268114404161094</v>
+        <v>0.26945906619803101</v>
       </c>
       <c r="F20" s="3">
-        <v>0.35409505396379848</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.30176930562416032</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="10"/>
-        <v>-0.30127472322825399</v>
-      </c>
-      <c r="K20" s="4">
-        <f t="shared" si="9"/>
-        <v>-0.39231215369103034</v>
-      </c>
-      <c r="L20" s="4">
-        <f>1-F20/F$18</f>
-        <v>-0.4195807730399217</v>
+        <v>0.43518880727046949</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="4"/>
+        <v>0.89093823970037622</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="L20" s="3">
+        <v>0.34505489318241123</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -1254,32 +1034,21 @@
         <v>10</v>
       </c>
       <c r="D21" s="3">
-        <v>0.21690102652958121</v>
+        <v>0.22469864149997759</v>
       </c>
       <c r="E21" s="3">
-        <v>0.14449349615565921</v>
+        <v>0.19358917771388709</v>
       </c>
       <c r="F21" s="3">
-        <v>0.23094762131043209</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0.1784192882457081</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="10"/>
-        <v>-9.8700762099446671E-2</v>
-      </c>
-      <c r="K21" s="4">
-        <f t="shared" si="9"/>
-        <v>0.24964847951266589</v>
-      </c>
-      <c r="L21" s="4">
-        <f t="shared" si="9"/>
-        <v>7.4122049654180011E-2</v>
+        <v>0.2756404923711705</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="4"/>
+        <v>8.5274835713573777E-2</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="L21" s="3">
+        <v>0.23358978481970519</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1293,71 +1062,49 @@
         <v>7</v>
       </c>
       <c r="D22" s="3">
-        <v>0.38115634267791237</v>
+        <v>0.39431943877960313</v>
       </c>
       <c r="E22" s="3">
-        <v>0.36481459222708729</v>
+        <v>0.36897011945494701</v>
       </c>
       <c r="F22" s="3">
-        <v>0.44685562793392752</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0.40394918932361229</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J22" s="4">
-        <f>1-D22/D$22</f>
+        <v>0.44804142689428827</v>
+      </c>
+      <c r="H22" s="4">
+        <f>ABS(D22-D$22)/D$22</f>
         <v>0</v>
       </c>
-      <c r="K22" s="4">
-        <f t="shared" ref="K22:L25" si="11">1-E22/E$22</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5">
+      <c r="I22" s="4"/>
+      <c r="L22" s="3">
+        <v>0.41136399328107781</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="7">
-        <v>0.57028678691437662</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0.4803033886324713</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0.6931527343221785</v>
-      </c>
-      <c r="H23" s="7">
-        <v>0.56972789096318488</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J23" s="8">
-        <f t="shared" ref="J23:J25" si="12">1-D23/D$22</f>
-        <v>-0.4962017499372553</v>
-      </c>
-      <c r="K23" s="8">
-        <f t="shared" si="11"/>
-        <v>-0.3165684675614493</v>
-      </c>
-      <c r="L23" s="8">
-        <f t="shared" si="11"/>
-        <v>-0.55117825756615213</v>
+      <c r="D23" s="3">
+        <v>0.44674987580908809</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.36646316456654321</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.4967078514455468</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" ref="H23:J25" si="5">ABS(D23-D$22)/D$22</f>
+        <v>0.13296437322936519</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="L23" s="3">
+        <v>0.42892219568534801</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1371,32 +1118,21 @@
         <v>9</v>
       </c>
       <c r="D24" s="3">
-        <v>0.44196137913623929</v>
+        <v>0.59580733530882801</v>
       </c>
       <c r="E24" s="3">
-        <v>0.242671125635293</v>
+        <v>0.5290353479735167</v>
       </c>
       <c r="F24" s="3">
-        <v>0.46929160429474931</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0.34886222961404861</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J24" s="4">
-        <f t="shared" si="12"/>
-        <v>-0.15952780958890878</v>
-      </c>
-      <c r="K24" s="4">
-        <f t="shared" si="11"/>
-        <v>0.33480970661327947</v>
-      </c>
-      <c r="L24" s="4">
-        <f t="shared" si="11"/>
-        <v>-5.0208557212440885E-2</v>
+        <v>0.71477709308543047</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="5"/>
+        <v>0.51097632202160459</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="L24" s="3">
+        <v>0.61191459270154436</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -1410,32 +1146,21 @@
         <v>10</v>
       </c>
       <c r="D25" s="3">
-        <v>0.40666046899736702</v>
+        <v>0.41106097454878748</v>
       </c>
       <c r="E25" s="3">
-        <v>0.39469106696020462</v>
+        <v>0.3589602043179792</v>
       </c>
       <c r="F25" s="3">
-        <v>0.62435751478277579</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.47892457635952768</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J25" s="4">
-        <f t="shared" si="12"/>
-        <v>-6.6912506663981519E-2</v>
-      </c>
-      <c r="K25" s="4">
-        <f t="shared" si="11"/>
-        <v>-8.1894955327115992E-2</v>
-      </c>
-      <c r="L25" s="4">
-        <f t="shared" si="11"/>
-        <v>-0.39722423922362204</v>
+        <v>0.4831729845250694</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="5"/>
+        <v>4.245678534387877E-2</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="L25" s="3">
+        <v>0.43427451280191859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major updates and fixes
</commit_message>
<xml_diff>
--- a/fermentation_insights/TRY_results/a_coeff_baselines_percentiles.xlsx
+++ b/fermentation_insights/TRY_results/a_coeff_baselines_percentiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
   <si>
     <t>product</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>TAL</t>
+  </si>
+  <si>
+    <t>TAL_SA</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>HP_neutral</t>
+  </si>
+  <si>
+    <t>HP_hexanol</t>
+  </si>
+  <si>
+    <t>HP_neutral_hexanol</t>
   </si>
   <si>
     <t>glucose</t>
@@ -404,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,19 +453,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>-0.02768889482627531</v>
       </c>
       <c r="E2">
-        <v>-0.2321243841912551</v>
+        <v>-0.1362040462341782</v>
       </c>
       <c r="F2">
-        <v>-0.07172026920198943</v>
+        <v>0.008068184414202694</v>
       </c>
       <c r="G2">
-        <v>0.1477771701526671</v>
+        <v>0.2082242651549941</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -461,19 +476,19 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>0.007173118460120858</v>
       </c>
       <c r="E3">
-        <v>-1.541721731506001</v>
+        <v>-0.3021664515059988</v>
       </c>
       <c r="F3">
-        <v>-1.068034181489867</v>
+        <v>-0.09120067291120472</v>
       </c>
       <c r="G3">
-        <v>-0.2722405274040913</v>
+        <v>0.1153356356138642</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,19 +499,19 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>0.1577408926958192</v>
       </c>
       <c r="E4">
-        <v>-0.2535390712012085</v>
+        <v>-0.04301282928242989</v>
       </c>
       <c r="F4">
-        <v>0.01198115568046577</v>
+        <v>0.204736975711393</v>
       </c>
       <c r="G4">
-        <v>0.2459788387629913</v>
+        <v>0.4378491752578832</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -507,19 +522,479 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>-0.03263376456909479</v>
       </c>
       <c r="E5">
-        <v>-0.5316354844526703</v>
+        <v>-0.3333023689334188</v>
       </c>
       <c r="F5">
-        <v>-0.2061860109491269</v>
+        <v>-0.04718585790564243</v>
       </c>
       <c r="G5">
-        <v>0.02783887678195665</v>
+        <v>0.1616025301881211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>1.693906493412831</v>
+      </c>
+      <c r="E6">
+        <v>1.376757598436993</v>
+      </c>
+      <c r="F6">
+        <v>1.779052365973022</v>
+      </c>
+      <c r="G6">
+        <v>2.215272123429149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>1.712425825792681</v>
+      </c>
+      <c r="E7">
+        <v>1.165038934676926</v>
+      </c>
+      <c r="F7">
+        <v>1.595040930973844</v>
+      </c>
+      <c r="G7">
+        <v>2.071442189097457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>2.569740436003511</v>
+      </c>
+      <c r="E8">
+        <v>1.89045243233971</v>
+      </c>
+      <c r="F8">
+        <v>2.611132524729333</v>
+      </c>
+      <c r="G8">
+        <v>3.575870592073538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>1.65935605110175</v>
+      </c>
+      <c r="E9">
+        <v>1.202388629267134</v>
+      </c>
+      <c r="F9">
+        <v>1.661695764817996</v>
+      </c>
+      <c r="G9">
+        <v>2.151201710178975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>0.1359449847057478</v>
+      </c>
+      <c r="E10">
+        <v>0.1217423275376321</v>
+      </c>
+      <c r="F10">
+        <v>0.1457881263552073</v>
+      </c>
+      <c r="G10">
+        <v>0.1746986175919518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>0.1251492020454104</v>
+      </c>
+      <c r="E11">
+        <v>0.1392624212582208</v>
+      </c>
+      <c r="F11">
+        <v>0.1644077639134778</v>
+      </c>
+      <c r="G11">
+        <v>0.1921672900576245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>0.2653195874577931</v>
+      </c>
+      <c r="E12">
+        <v>0.2252919992696443</v>
+      </c>
+      <c r="F12">
+        <v>0.2888034213529128</v>
+      </c>
+      <c r="G12">
+        <v>0.381762496107142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0.1457077863321944</v>
+      </c>
+      <c r="E13">
+        <v>0.1500656055288403</v>
+      </c>
+      <c r="F13">
+        <v>0.1742492459529436</v>
+      </c>
+      <c r="G13">
+        <v>0.2017454321808168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0.322119202608785</v>
+      </c>
+      <c r="E14">
+        <v>0.2936933754843657</v>
+      </c>
+      <c r="F14">
+        <v>0.3321613417160705</v>
+      </c>
+      <c r="G14">
+        <v>0.3709695397782817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>0.3113482406964271</v>
+      </c>
+      <c r="E15">
+        <v>0.3189608061335971</v>
+      </c>
+      <c r="F15">
+        <v>0.3590901546239755</v>
+      </c>
+      <c r="G15">
+        <v>0.3972962375812892</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>0.460612553989721</v>
+      </c>
+      <c r="E16">
+        <v>0.4157954471826902</v>
+      </c>
+      <c r="F16">
+        <v>0.488107581258493</v>
+      </c>
+      <c r="G16">
+        <v>0.5802806535003453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0.3346891061168057</v>
+      </c>
+      <c r="E17">
+        <v>0.3258815608406543</v>
+      </c>
+      <c r="F17">
+        <v>0.3654391001968582</v>
+      </c>
+      <c r="G17">
+        <v>0.4039684429524503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>0.222630461415264</v>
+      </c>
+      <c r="E18">
+        <v>0.2049276796397576</v>
+      </c>
+      <c r="F18">
+        <v>0.2332493769655308</v>
+      </c>
+      <c r="G18">
+        <v>0.2653060149405092</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>0.2656214605396013</v>
+      </c>
+      <c r="E19">
+        <v>0.2932285614427803</v>
+      </c>
+      <c r="F19">
+        <v>0.3304452859023807</v>
+      </c>
+      <c r="G19">
+        <v>0.371341372484722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>0.4329267584633505</v>
+      </c>
+      <c r="E20">
+        <v>0.3761378850958221</v>
+      </c>
+      <c r="F20">
+        <v>0.4492190274544461</v>
+      </c>
+      <c r="G20">
+        <v>0.5561386505531415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>0.2404864593225714</v>
+      </c>
+      <c r="E21">
+        <v>0.2523260370675316</v>
+      </c>
+      <c r="F21">
+        <v>0.2805876367084105</v>
+      </c>
+      <c r="G21">
+        <v>0.3126885330573852</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>0.4090175567162433</v>
+      </c>
+      <c r="E22">
+        <v>0.3737226091252088</v>
+      </c>
+      <c r="F22">
+        <v>0.4146976412877547</v>
+      </c>
+      <c r="G22">
+        <v>0.4574331199615876</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>0.4436055105672664</v>
+      </c>
+      <c r="E23">
+        <v>0.4695942673050749</v>
+      </c>
+      <c r="F23">
+        <v>0.5144215484823791</v>
+      </c>
+      <c r="G23">
+        <v>0.5648386490224796</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>0.6329256430259</v>
+      </c>
+      <c r="E24">
+        <v>0.5631330558455231</v>
+      </c>
+      <c r="F24">
+        <v>0.6420724353615753</v>
+      </c>
+      <c r="G24">
+        <v>0.7571931234683505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>0.4265117601073674</v>
+      </c>
+      <c r="E25">
+        <v>0.4191620793821572</v>
+      </c>
+      <c r="F25">
+        <v>0.4615748737559754</v>
+      </c>
+      <c r="G25">
+        <v>0.5025401378537185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>